<commit_message>
update engine to be more generic
</commit_message>
<xml_diff>
--- a/sample/Primary.xlsx
+++ b/sample/Primary.xlsx
@@ -410,22 +410,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1">
         <f>[1]Feuil1!$A$1+[1]Feuil1!$B$1+[1]Feuil1!$C$1</f>
         <v>42</v>
       </c>
       <c r="B1">
-        <f>A1+2</f>
-        <v>44</v>
+        <f>A1+2+C1</f>
+        <v>42</v>
+      </c>
+      <c r="C1">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>